<commit_message>
cleaning up iptds website
</commit_message>
<xml_diff>
--- a/data/prioritization/iptds_site_recommendations_20241211.xlsx
+++ b/data/prioritization/iptds_site_recommendations_20241211.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\prioritization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBD095B-F801-44DF-97D6-DE171AB6305C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7186EF0B-F34D-4BED-80F1-8B0759A3E623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -830,7 +830,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E51" sqref="E2:E51"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1346,7 +1346,7 @@
         <v>-115.56588600000001</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1363,7 +1363,7 @@
         <v>-115.515533</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>145</v>
@@ -1689,7 +1689,7 @@
         <v>-117.579223</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1706,7 +1706,7 @@
         <v>-117.72657</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
just saving some file changes while drafting iptds implementation plan
</commit_message>
<xml_diff>
--- a/data/prioritization/iptds_site_recommendations_20241211.xlsx
+++ b/data/prioritization/iptds_site_recommendations_20241211.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\prioritization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF999226-F7F9-4B84-9C73-006EF97829B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C05BDAA-7DCC-40B1-9218-44B533325E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -830,7 +830,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1765,7 +1765,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F51" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
noted that LLR was recently upgraded to IS1001 MC
</commit_message>
<xml_diff>
--- a/data/prioritization/iptds_site_recommendations_20241211.xlsx
+++ b/data/prioritization/iptds_site_recommendations_20241211.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\prioritization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C05BDAA-7DCC-40B1-9218-44B533325E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B6073F-32FC-420F-BE8C-22FADE297A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,9 +445,6 @@
     <t>When removed, any usable infrastructure could be relocated to proposed USC, EFS, and/or USP locations.</t>
   </si>
   <si>
-    <t>Long-term, consider upgrades to IS1001 to increase read range. During upgrades, could be considered for consolidation to a single-pass array.</t>
-  </si>
-  <si>
     <t>Evaluate feasibility of an IPTDS in SRCHA-s and SRCHA populations. Preferred locations would be lower Chamberlain Creek. Alternate locations: upper Chamberlain, Sabe, Bargamin, Warren, Crooked, or Sheep creeks. Any of the proposed locations would need to be a tandem array.</t>
   </si>
   <si>
@@ -479,6 +476,9 @@
   </si>
   <si>
     <t>Long-term, if desired, SW2 could be moved to the end of the Selway Road which would allow parsing of the SEMOO and SEUMA Chinook salmon populations from SEMEA, but would need to be a tandem array.</t>
+  </si>
+  <si>
+    <t>Recently upgraded to a IS1001 Master Controller.</t>
   </si>
 </sst>
 </file>
@@ -830,7 +830,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1016,7 +1016,7 @@
         <v>117</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1172,7 +1172,7 @@
         <v>119</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1275,7 +1275,7 @@
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1295,7 +1295,7 @@
         <v>119</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1366,7 +1366,7 @@
         <v>119</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1431,7 +1431,7 @@
         <v>119</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1451,7 +1451,7 @@
         <v>117</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1471,7 +1471,7 @@
         <v>117</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1506,7 +1506,7 @@
         <v>117</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1526,7 +1526,7 @@
         <v>117</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1652,7 +1652,7 @@
         <v>117</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1672,7 +1672,7 @@
         <v>118</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1761,7 +1761,7 @@
         <v>117</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated priority for ACM on map
</commit_message>
<xml_diff>
--- a/data/prioritization/iptds_site_recommendations_20241211.xlsx
+++ b/data/prioritization/iptds_site_recommendations_20241211.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\prioritization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD98F66B-1881-4E95-B8E6-9565E9AC4132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AC99D1-44F7-4920-B7FF-8984A837096B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -830,7 +830,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1758,7 +1758,7 @@
         <v>-117.055707</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>143</v>

</xml_diff>